<commit_message>
feat: :sparkles: testes realizados, algorítimo pronto para uso
</commit_message>
<xml_diff>
--- a/IPD/salvo.xlsx
+++ b/IPD/salvo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>intervalo</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ordem</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -456,6 +461,9 @@
           <t>1H - 2H</t>
         </is>
       </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -468,6 +476,9 @@
           <t>2H - 3H</t>
         </is>
       </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -480,6 +491,9 @@
           <t>3H - 4H</t>
         </is>
       </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -492,6 +506,9 @@
           <t>4H - 6H</t>
         </is>
       </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -504,6 +521,9 @@
           <t>6H - 7H</t>
         </is>
       </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -516,6 +536,9 @@
           <t>7H - 12H</t>
         </is>
       </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -528,6 +551,9 @@
           <t>12H - 22H</t>
         </is>
       </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -540,6 +566,9 @@
           <t>22H - 23H</t>
         </is>
       </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -552,6 +581,9 @@
           <t>23H - 1H</t>
         </is>
       </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -564,6 +596,9 @@
           <t>1H - 2H</t>
         </is>
       </c>
+      <c r="C11" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -576,6 +611,9 @@
           <t>2H - 3H</t>
         </is>
       </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -588,6 +626,9 @@
           <t>3H - 4H</t>
         </is>
       </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -600,6 +641,9 @@
           <t>23H - 1H</t>
         </is>
       </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -612,6 +656,9 @@
           <t>3H - 4H</t>
         </is>
       </c>
+      <c r="C15" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -624,6 +671,9 @@
           <t>4H - 6H</t>
         </is>
       </c>
+      <c r="C16" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -636,6 +686,9 @@
           <t>23H - 1H</t>
         </is>
       </c>
+      <c r="C17" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -648,6 +701,9 @@
           <t>7H - 12H</t>
         </is>
       </c>
+      <c r="C18" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -660,6 +716,9 @@
           <t>23H - 1H</t>
         </is>
       </c>
+      <c r="C19" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -672,6 +731,9 @@
           <t>12H - 22H</t>
         </is>
       </c>
+      <c r="C20" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -684,6 +746,9 @@
           <t>22H - 23H</t>
         </is>
       </c>
+      <c r="C21" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -696,6 +761,9 @@
           <t>23H - 1H</t>
         </is>
       </c>
+      <c r="C22" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -708,6 +776,9 @@
           <t>4H - 6H</t>
         </is>
       </c>
+      <c r="C23" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -720,6 +791,9 @@
           <t>6H - 7H</t>
         </is>
       </c>
+      <c r="C24" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -732,6 +806,9 @@
           <t>7H - 12H</t>
         </is>
       </c>
+      <c r="C25" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -744,6 +821,9 @@
           <t>12H - 22H</t>
         </is>
       </c>
+      <c r="C26" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -756,6 +836,9 @@
           <t>22H - 23H</t>
         </is>
       </c>
+      <c r="C27" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -768,6 +851,9 @@
           <t>23H - 1H</t>
         </is>
       </c>
+      <c r="C28" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -780,6 +866,9 @@
           <t>1H - 2H</t>
         </is>
       </c>
+      <c r="C29" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -792,6 +881,9 @@
           <t>23H - 1H</t>
         </is>
       </c>
+      <c r="C30" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -804,6 +896,9 @@
           <t>4H - 6H</t>
         </is>
       </c>
+      <c r="C31" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -816,6 +911,9 @@
           <t>23H - 1H</t>
         </is>
       </c>
+      <c r="C32" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -828,6 +926,9 @@
           <t>4H - 6H</t>
         </is>
       </c>
+      <c r="C33" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -840,6 +941,9 @@
           <t>6H - 7H</t>
         </is>
       </c>
+      <c r="C34" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -852,6 +956,9 @@
           <t>7H - 12H</t>
         </is>
       </c>
+      <c r="C35" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -864,6 +971,9 @@
           <t>12H - 22H</t>
         </is>
       </c>
+      <c r="C36" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -876,6 +986,9 @@
           <t>23H - 1H</t>
         </is>
       </c>
+      <c r="C37" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -888,6 +1001,9 @@
           <t>1H - 2H</t>
         </is>
       </c>
+      <c r="C38" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -900,6 +1016,9 @@
           <t>2H - 3H</t>
         </is>
       </c>
+      <c r="C39" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -912,6 +1031,9 @@
           <t>3H - 4H</t>
         </is>
       </c>
+      <c r="C40" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -923,6 +1045,9 @@
         <is>
           <t>23H - 1H</t>
         </is>
+      </c>
+      <c r="C41" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>